<commit_message>
Add changes to generate SW configurations for Landry
</commit_message>
<xml_diff>
--- a/2.bioemus configuration scripts/input config/inputConfigs.xlsx
+++ b/2.bioemus configuration scripts/input config/inputConfigs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bioemus-pyscripts\input config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arianna\Documents\gdvMT\gdvMT\2.bioemus configuration scripts\input config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B395081-73B1-4961-9EA4-DC7AB1D6C591}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE5646C-C6D2-448F-ADC3-4D4D48DAEA4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="14">
   <si>
     <t># CONFIG</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>50/50</t>
+  </si>
+  <si>
+    <t>250519_5</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D271"/>
+  <dimension ref="A1:D274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:XFD89"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,8 +421,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1056</v>
+      <c r="A2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -432,39 +435,39 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1057</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2.5499999999999998E-2</v>
+      <c r="A3" s="2">
+        <v>1324</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.5700000000000001E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1058</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2.5499999999999998E-2</v>
+      <c r="A4" s="2">
+        <v>1325</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2.5700000000000001E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -475,13 +478,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
         <v>2.5499999999999998E-2</v>
@@ -489,13 +492,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
         <v>2.5499999999999998E-2</v>
@@ -503,13 +506,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
         <v>2.5499999999999998E-2</v>
@@ -517,10 +520,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C9" s="1">
         <v>0.5</v>
@@ -531,13 +534,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D10" s="1">
         <v>2.5499999999999998E-2</v>
@@ -545,13 +548,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="1">
         <v>2.5499999999999998E-2</v>
@@ -559,13 +562,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="1">
         <v>2.5499999999999998E-2</v>
@@ -573,10 +576,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1">
         <v>0.75</v>
@@ -587,13 +590,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D14" s="1">
         <v>2.5499999999999998E-2</v>
@@ -601,13 +604,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D15" s="1">
         <v>2.5499999999999998E-2</v>
@@ -615,13 +618,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="1">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D16" s="1">
         <v>2.5499999999999998E-2</v>
@@ -629,10 +632,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1">
         <v>0.1</v>
@@ -643,13 +646,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D18" s="1">
         <v>2.5499999999999998E-2</v>
@@ -657,13 +660,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D19" s="1">
         <v>2.5499999999999998E-2</v>
@@ -671,13 +674,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C20" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D20" s="1">
         <v>2.5499999999999998E-2</v>
@@ -685,10 +688,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C21" s="1">
         <v>0.25</v>
@@ -699,13 +702,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D22" s="1">
         <v>2.5499999999999998E-2</v>
@@ -713,13 +716,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D23" s="1">
         <v>2.5499999999999998E-2</v>
@@ -727,13 +730,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D24" s="1">
         <v>2.5499999999999998E-2</v>
@@ -741,10 +744,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C25" s="1">
         <v>0.4</v>
@@ -755,13 +758,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C26" s="1">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D26" s="1">
         <v>2.5499999999999998E-2</v>
@@ -769,13 +772,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D27" s="1">
         <v>2.5499999999999998E-2</v>
@@ -783,13 +786,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D28" s="1">
         <v>2.5499999999999998E-2</v>
@@ -797,13 +800,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1">
         <v>2.5499999999999998E-2</v>
@@ -811,13 +814,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D30" s="1">
         <v>2.5499999999999998E-2</v>
@@ -825,13 +828,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="1">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D31" s="1">
         <v>2.5499999999999998E-2</v>
@@ -839,13 +842,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D32" s="1">
         <v>2.5499999999999998E-2</v>
@@ -853,13 +856,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="1">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D33" s="1">
         <v>2.5499999999999998E-2</v>
@@ -867,13 +870,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34" s="1">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D34" s="1">
         <v>2.5499999999999998E-2</v>
@@ -881,13 +884,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C35" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1">
         <v>2.5499999999999998E-2</v>
@@ -895,13 +898,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D36" s="1">
         <v>2.5499999999999998E-2</v>
@@ -909,13 +912,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C37" s="1">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D37" s="1">
         <v>2.5499999999999998E-2</v>
@@ -923,13 +926,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C38" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D38" s="1">
         <v>2.5499999999999998E-2</v>
@@ -937,13 +940,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C39" s="1">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D39" s="1">
         <v>2.5499999999999998E-2</v>
@@ -951,13 +954,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" s="1">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D40" s="1">
         <v>2.5499999999999998E-2</v>
@@ -965,13 +968,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C41" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D41" s="1">
         <v>2.5499999999999998E-2</v>
@@ -979,13 +982,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D42" s="1">
         <v>2.5499999999999998E-2</v>
@@ -993,13 +996,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C43" s="1">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D43" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1007,13 +1010,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D44" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1021,13 +1024,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C45" s="1">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D45" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1035,13 +1038,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C46" s="1">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D46" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1049,13 +1052,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1063,13 +1066,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D48" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1077,13 +1080,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="1">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D49" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1091,13 +1094,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C50" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D50" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1105,13 +1108,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51" s="1">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D51" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1119,13 +1122,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C52" s="1">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D52" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1133,13 +1136,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C53" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1147,13 +1150,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D54" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1161,13 +1164,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C55" s="1">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D55" s="1">
         <v>2.5499999999999998E-2</v>
@@ -1175,52 +1178,52 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C56" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D56" s="1">
-        <v>2.5600000000000001E-2</v>
+        <v>2.5499999999999998E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C57" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D57" s="1">
-        <v>2.5600000000000001E-2</v>
+        <v>2.5499999999999998E-2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C58" s="1">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D58" s="1">
-        <v>2.5600000000000001E-2</v>
+        <v>2.5499999999999998E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
@@ -1231,13 +1234,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C60" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D60" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1245,13 +1248,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C61" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D61" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1259,13 +1262,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C62" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D62" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1273,10 +1276,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1">
         <v>0.5</v>
@@ -1287,13 +1290,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D64" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1301,13 +1304,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C65" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D65" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1315,13 +1318,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C66" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D66" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1329,10 +1332,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C67" s="1">
         <v>0.75</v>
@@ -1343,13 +1346,13 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C68" s="1">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D68" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1357,13 +1360,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C69" s="1">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D69" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1371,13 +1374,13 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C70" s="1">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D70" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1385,10 +1388,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C71" s="1">
         <v>0.1</v>
@@ -1399,13 +1402,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C72" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D72" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1413,13 +1416,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C73" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D73" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1427,13 +1430,13 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C74" s="1">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D74" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1441,10 +1444,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C75" s="1">
         <v>0.25</v>
@@ -1455,13 +1458,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D76" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1469,13 +1472,13 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C77" s="1">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D77" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1483,13 +1486,13 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C78" s="1">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D78" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1497,10 +1500,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C79" s="1">
         <v>0.4</v>
@@ -1511,13 +1514,13 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C80" s="1">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D80" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1525,13 +1528,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C81" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D81" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1539,13 +1542,13 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C82" s="1">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D82" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1553,13 +1556,13 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C83" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D83" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1567,13 +1570,13 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C84" s="1">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D84" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1581,13 +1584,13 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C85" s="1">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D85" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1595,13 +1598,13 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C86" s="1">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D86" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1609,13 +1612,13 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C87" s="1">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D87" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1623,13 +1626,13 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C88" s="1">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D88" s="1">
         <v>2.5600000000000001E-2</v>
@@ -1637,69 +1640,69 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C89" s="1">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D89" s="1">
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="90" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>1144</v>
-      </c>
-      <c r="B90" s="2" t="s">
+      <c r="A90" s="1">
+        <v>1141</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C90" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D90" s="2">
+      <c r="C90" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D90" s="1">
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
-        <v>1145</v>
-      </c>
-      <c r="B91" s="2" t="s">
+      <c r="A91" s="1">
+        <v>1142</v>
+      </c>
+      <c r="B91" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C91" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="D91" s="2">
+      <c r="C91" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D91" s="1">
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="92" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>1146</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" s="2">
-        <v>1</v>
-      </c>
-      <c r="D92" s="2">
+      <c r="A92" s="1">
+        <v>1143</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="D92" s="1">
         <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C93" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D93" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1707,13 +1710,13 @@
     </row>
     <row r="94" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C94" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D94" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1721,13 +1724,13 @@
     </row>
     <row r="95" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C95" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D95" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1735,13 +1738,13 @@
     </row>
     <row r="96" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C96" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D96" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1749,13 +1752,13 @@
     </row>
     <row r="97" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C97" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D97" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1763,13 +1766,13 @@
     </row>
     <row r="98" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C98" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D98" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1777,13 +1780,13 @@
     </row>
     <row r="99" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C99" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D99" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1791,13 +1794,13 @@
     </row>
     <row r="100" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C100" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D100" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1805,13 +1808,13 @@
     </row>
     <row r="101" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C101" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D101" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1819,13 +1822,13 @@
     </row>
     <row r="102" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C102" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D102" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1833,13 +1836,13 @@
     </row>
     <row r="103" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C103" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D103" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1847,13 +1850,13 @@
     </row>
     <row r="104" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C104" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D104" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1861,13 +1864,13 @@
     </row>
     <row r="105" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C105" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D105" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1875,13 +1878,13 @@
     </row>
     <row r="106" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C106" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D106" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1889,13 +1892,13 @@
     </row>
     <row r="107" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C107" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D107" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1903,13 +1906,13 @@
     </row>
     <row r="108" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C108" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D108" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1917,13 +1920,13 @@
     </row>
     <row r="109" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C109" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D109" s="2">
         <v>2.5600000000000001E-2</v>
@@ -1931,52 +1934,52 @@
     </row>
     <row r="110" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C110" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D110" s="2">
-        <v>2.555E-2</v>
+        <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="111" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C111" s="2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D111" s="2">
-        <v>2.555E-2</v>
+        <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="112" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C112" s="2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D112" s="2">
-        <v>2.555E-2</v>
+        <v>2.5600000000000001E-2</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C113" s="2">
         <v>1</v>
@@ -1987,13 +1990,13 @@
     </row>
     <row r="114" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C114" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D114" s="2">
         <v>2.555E-2</v>
@@ -2001,13 +2004,13 @@
     </row>
     <row r="115" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C115" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D115" s="2">
         <v>2.555E-2</v>
@@ -2015,13 +2018,13 @@
     </row>
     <row r="116" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C116" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D116" s="2">
         <v>2.555E-2</v>
@@ -2029,10 +2032,10 @@
     </row>
     <row r="117" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C117" s="2">
         <v>0.5</v>
@@ -2043,13 +2046,13 @@
     </row>
     <row r="118" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C118" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D118" s="2">
         <v>2.555E-2</v>
@@ -2057,13 +2060,13 @@
     </row>
     <row r="119" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C119" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D119" s="2">
         <v>2.555E-2</v>
@@ -2071,13 +2074,13 @@
     </row>
     <row r="120" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C120" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D120" s="2">
         <v>2.555E-2</v>
@@ -2085,10 +2088,10 @@
     </row>
     <row r="121" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C121" s="2">
         <v>0.75</v>
@@ -2099,13 +2102,13 @@
     </row>
     <row r="122" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C122" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D122" s="2">
         <v>2.555E-2</v>
@@ -2113,13 +2116,13 @@
     </row>
     <row r="123" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C123" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D123" s="2">
         <v>2.555E-2</v>
@@ -2127,13 +2130,13 @@
     </row>
     <row r="124" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C124" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D124" s="2">
         <v>2.555E-2</v>
@@ -2141,10 +2144,10 @@
     </row>
     <row r="125" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C125" s="2">
         <v>0.1</v>
@@ -2155,13 +2158,13 @@
     </row>
     <row r="126" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C126" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D126" s="2">
         <v>2.555E-2</v>
@@ -2169,13 +2172,13 @@
     </row>
     <row r="127" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C127" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D127" s="2">
         <v>2.555E-2</v>
@@ -2183,13 +2186,13 @@
     </row>
     <row r="128" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C128" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D128" s="2">
         <v>2.555E-2</v>
@@ -2197,10 +2200,10 @@
     </row>
     <row r="129" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C129" s="2">
         <v>0.25</v>
@@ -2211,13 +2214,13 @@
     </row>
     <row r="130" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C130" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D130" s="2">
         <v>2.555E-2</v>
@@ -2225,13 +2228,13 @@
     </row>
     <row r="131" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C131" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D131" s="2">
         <v>2.555E-2</v>
@@ -2239,13 +2242,13 @@
     </row>
     <row r="132" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C132" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D132" s="2">
         <v>2.555E-2</v>
@@ -2253,10 +2256,10 @@
     </row>
     <row r="133" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C133" s="2">
         <v>0.4</v>
@@ -2267,13 +2270,13 @@
     </row>
     <row r="134" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C134" s="2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D134" s="2">
         <v>2.555E-2</v>
@@ -2281,13 +2284,13 @@
     </row>
     <row r="135" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C135" s="2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D135" s="2">
         <v>2.555E-2</v>
@@ -2295,13 +2298,13 @@
     </row>
     <row r="136" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C136" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D136" s="2">
         <v>2.555E-2</v>
@@ -2309,13 +2312,13 @@
     </row>
     <row r="137" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C137" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D137" s="2">
         <v>2.555E-2</v>
@@ -2323,13 +2326,13 @@
     </row>
     <row r="138" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C138" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D138" s="2">
         <v>2.555E-2</v>
@@ -2337,13 +2340,13 @@
     </row>
     <row r="139" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C139" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D139" s="2">
         <v>2.555E-2</v>
@@ -2351,13 +2354,13 @@
     </row>
     <row r="140" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C140" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D140" s="2">
         <v>2.555E-2</v>
@@ -2365,13 +2368,13 @@
     </row>
     <row r="141" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>1195</v>
+        <v>1192</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C141" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D141" s="2">
         <v>2.555E-2</v>
@@ -2379,13 +2382,13 @@
     </row>
     <row r="142" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C142" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D142" s="2">
         <v>2.555E-2</v>
@@ -2393,13 +2396,13 @@
     </row>
     <row r="143" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C143" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D143" s="2">
         <v>2.555E-2</v>
@@ -2407,13 +2410,13 @@
     </row>
     <row r="144" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C144" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D144" s="2">
         <v>2.555E-2</v>
@@ -2421,13 +2424,13 @@
     </row>
     <row r="145" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C145" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D145" s="2">
         <v>2.555E-2</v>
@@ -2435,13 +2438,13 @@
     </row>
     <row r="146" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C146" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D146" s="2">
         <v>2.555E-2</v>
@@ -2449,13 +2452,13 @@
     </row>
     <row r="147" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C147" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D147" s="2">
         <v>2.555E-2</v>
@@ -2463,13 +2466,13 @@
     </row>
     <row r="148" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C148" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D148" s="2">
         <v>2.555E-2</v>
@@ -2477,13 +2480,13 @@
     </row>
     <row r="149" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C149" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D149" s="2">
         <v>2.555E-2</v>
@@ -2491,13 +2494,13 @@
     </row>
     <row r="150" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C150" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D150" s="2">
         <v>2.555E-2</v>
@@ -2505,13 +2508,13 @@
     </row>
     <row r="151" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="B151" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C151" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D151" s="2">
         <v>2.555E-2</v>
@@ -2519,13 +2522,13 @@
     </row>
     <row r="152" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C152" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D152" s="2">
         <v>2.555E-2</v>
@@ -2533,13 +2536,13 @@
     </row>
     <row r="153" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C153" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D153" s="2">
         <v>2.555E-2</v>
@@ -2547,13 +2550,13 @@
     </row>
     <row r="154" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C154" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D154" s="2">
         <v>2.555E-2</v>
@@ -2561,13 +2564,13 @@
     </row>
     <row r="155" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="B155" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C155" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D155" s="2">
         <v>2.555E-2</v>
@@ -2575,13 +2578,13 @@
     </row>
     <row r="156" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C156" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D156" s="2">
         <v>2.555E-2</v>
@@ -2589,13 +2592,13 @@
     </row>
     <row r="157" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="B157" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C157" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D157" s="2">
         <v>2.555E-2</v>
@@ -2603,13 +2606,13 @@
     </row>
     <row r="158" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C158" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D158" s="2">
         <v>2.555E-2</v>
@@ -2617,13 +2620,13 @@
     </row>
     <row r="159" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C159" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D159" s="2">
         <v>2.555E-2</v>
@@ -2631,13 +2634,13 @@
     </row>
     <row r="160" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C160" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D160" s="2">
         <v>2.555E-2</v>
@@ -2645,13 +2648,13 @@
     </row>
     <row r="161" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="B161" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C161" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D161" s="2">
         <v>2.555E-2</v>
@@ -2659,13 +2662,13 @@
     </row>
     <row r="162" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="B162" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C162" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D162" s="2">
         <v>2.555E-2</v>
@@ -2673,13 +2676,13 @@
     </row>
     <row r="163" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="B163" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C163" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D163" s="2">
         <v>2.555E-2</v>
@@ -2687,52 +2690,52 @@
     </row>
     <row r="164" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C164" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D164" s="2">
-        <v>2.545E-2</v>
+        <v>2.555E-2</v>
       </c>
     </row>
     <row r="165" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>1219</v>
+        <v>1216</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C165" s="2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D165" s="2">
-        <v>2.545E-2</v>
+        <v>2.555E-2</v>
       </c>
     </row>
     <row r="166" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>1220</v>
+        <v>1217</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C166" s="2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D166" s="2">
-        <v>2.545E-2</v>
+        <v>2.555E-2</v>
       </c>
     </row>
     <row r="167" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C167" s="2">
         <v>1</v>
@@ -2743,13 +2746,13 @@
     </row>
     <row r="168" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C168" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D168" s="2">
         <v>2.545E-2</v>
@@ -2757,13 +2760,13 @@
     </row>
     <row r="169" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C169" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D169" s="2">
         <v>2.545E-2</v>
@@ -2771,13 +2774,13 @@
     </row>
     <row r="170" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C170" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D170" s="2">
         <v>2.545E-2</v>
@@ -2785,10 +2788,10 @@
     </row>
     <row r="171" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C171" s="2">
         <v>0.5</v>
@@ -2799,13 +2802,13 @@
     </row>
     <row r="172" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C172" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D172" s="2">
         <v>2.545E-2</v>
@@ -2813,13 +2816,13 @@
     </row>
     <row r="173" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C173" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D173" s="2">
         <v>2.545E-2</v>
@@ -2827,13 +2830,13 @@
     </row>
     <row r="174" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C174" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D174" s="2">
         <v>2.545E-2</v>
@@ -2841,10 +2844,10 @@
     </row>
     <row r="175" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C175" s="2">
         <v>0.75</v>
@@ -2855,13 +2858,13 @@
     </row>
     <row r="176" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C176" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D176" s="2">
         <v>2.545E-2</v>
@@ -2869,13 +2872,13 @@
     </row>
     <row r="177" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C177" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D177" s="2">
         <v>2.545E-2</v>
@@ -2883,13 +2886,13 @@
     </row>
     <row r="178" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C178" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D178" s="2">
         <v>2.545E-2</v>
@@ -2897,10 +2900,10 @@
     </row>
     <row r="179" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C179" s="2">
         <v>0.1</v>
@@ -2911,13 +2914,13 @@
     </row>
     <row r="180" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C180" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D180" s="2">
         <v>2.545E-2</v>
@@ -2925,13 +2928,13 @@
     </row>
     <row r="181" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C181" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D181" s="2">
         <v>2.545E-2</v>
@@ -2939,13 +2942,13 @@
     </row>
     <row r="182" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C182" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D182" s="2">
         <v>2.545E-2</v>
@@ -2953,10 +2956,10 @@
     </row>
     <row r="183" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C183" s="2">
         <v>0.25</v>
@@ -2967,13 +2970,13 @@
     </row>
     <row r="184" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C184" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D184" s="2">
         <v>2.545E-2</v>
@@ -2981,13 +2984,13 @@
     </row>
     <row r="185" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C185" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D185" s="2">
         <v>2.545E-2</v>
@@ -2995,13 +2998,13 @@
     </row>
     <row r="186" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C186" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D186" s="2">
         <v>2.545E-2</v>
@@ -3009,10 +3012,10 @@
     </row>
     <row r="187" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C187" s="2">
         <v>0.4</v>
@@ -3023,13 +3026,13 @@
     </row>
     <row r="188" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C188" s="2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D188" s="2">
         <v>2.545E-2</v>
@@ -3037,13 +3040,13 @@
     </row>
     <row r="189" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C189" s="2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D189" s="2">
         <v>2.545E-2</v>
@@ -3051,13 +3054,13 @@
     </row>
     <row r="190" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C190" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D190" s="2">
         <v>2.545E-2</v>
@@ -3065,13 +3068,13 @@
     </row>
     <row r="191" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C191" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D191" s="2">
         <v>2.545E-2</v>
@@ -3079,13 +3082,13 @@
     </row>
     <row r="192" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C192" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D192" s="2">
         <v>2.545E-2</v>
@@ -3093,13 +3096,13 @@
     </row>
     <row r="193" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C193" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D193" s="2">
         <v>2.545E-2</v>
@@ -3107,13 +3110,13 @@
     </row>
     <row r="194" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C194" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D194" s="2">
         <v>2.545E-2</v>
@@ -3121,13 +3124,13 @@
     </row>
     <row r="195" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C195" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D195" s="2">
         <v>2.545E-2</v>
@@ -3135,13 +3138,13 @@
     </row>
     <row r="196" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C196" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D196" s="2">
         <v>2.545E-2</v>
@@ -3149,13 +3152,13 @@
     </row>
     <row r="197" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C197" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D197" s="2">
         <v>2.545E-2</v>
@@ -3163,13 +3166,13 @@
     </row>
     <row r="198" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C198" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D198" s="2">
         <v>2.545E-2</v>
@@ -3177,13 +3180,13 @@
     </row>
     <row r="199" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C199" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D199" s="2">
         <v>2.545E-2</v>
@@ -3191,13 +3194,13 @@
     </row>
     <row r="200" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C200" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D200" s="2">
         <v>2.545E-2</v>
@@ -3205,13 +3208,13 @@
     </row>
     <row r="201" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C201" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D201" s="2">
         <v>2.545E-2</v>
@@ -3219,13 +3222,13 @@
     </row>
     <row r="202" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C202" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D202" s="2">
         <v>2.545E-2</v>
@@ -3233,13 +3236,13 @@
     </row>
     <row r="203" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C203" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D203" s="2">
         <v>2.545E-2</v>
@@ -3247,13 +3250,13 @@
     </row>
     <row r="204" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C204" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D204" s="2">
         <v>2.545E-2</v>
@@ -3261,13 +3264,13 @@
     </row>
     <row r="205" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C205" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D205" s="2">
         <v>2.545E-2</v>
@@ -3275,13 +3278,13 @@
     </row>
     <row r="206" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C206" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D206" s="2">
         <v>2.545E-2</v>
@@ -3289,13 +3292,13 @@
     </row>
     <row r="207" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C207" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D207" s="2">
         <v>2.545E-2</v>
@@ -3303,13 +3306,13 @@
     </row>
     <row r="208" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C208" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D208" s="2">
         <v>2.545E-2</v>
@@ -3317,13 +3320,13 @@
     </row>
     <row r="209" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C209" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D209" s="2">
         <v>2.545E-2</v>
@@ -3331,13 +3334,13 @@
     </row>
     <row r="210" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C210" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D210" s="2">
         <v>2.545E-2</v>
@@ -3345,13 +3348,13 @@
     </row>
     <row r="211" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C211" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D211" s="2">
         <v>2.545E-2</v>
@@ -3359,13 +3362,13 @@
     </row>
     <row r="212" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C212" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D212" s="2">
         <v>2.545E-2</v>
@@ -3373,13 +3376,13 @@
     </row>
     <row r="213" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C213" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D213" s="2">
         <v>2.545E-2</v>
@@ -3387,13 +3390,13 @@
     </row>
     <row r="214" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C214" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D214" s="2">
         <v>2.545E-2</v>
@@ -3401,13 +3404,13 @@
     </row>
     <row r="215" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C215" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D215" s="2">
         <v>2.545E-2</v>
@@ -3415,13 +3418,13 @@
     </row>
     <row r="216" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C216" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D216" s="2">
         <v>2.545E-2</v>
@@ -3429,13 +3432,13 @@
     </row>
     <row r="217" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C217" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D217" s="2">
         <v>2.545E-2</v>
@@ -3443,52 +3446,52 @@
     </row>
     <row r="218" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C218" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D218" s="2">
-        <v>2.5700000000000001E-2</v>
+        <v>2.545E-2</v>
       </c>
     </row>
     <row r="219" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C219" s="2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D219" s="2">
-        <v>2.5700000000000001E-2</v>
+        <v>2.545E-2</v>
       </c>
     </row>
     <row r="220" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C220" s="2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D220" s="2">
-        <v>2.5700000000000001E-2</v>
+        <v>2.545E-2</v>
       </c>
     </row>
     <row r="221" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C221" s="2">
         <v>1</v>
@@ -3499,13 +3502,13 @@
     </row>
     <row r="222" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C222" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D222" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3513,13 +3516,13 @@
     </row>
     <row r="223" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
-        <v>1277</v>
+        <v>1274</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C223" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D223" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3527,13 +3530,13 @@
     </row>
     <row r="224" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
-        <v>1278</v>
+        <v>1275</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C224" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D224" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3541,10 +3544,10 @@
     </row>
     <row r="225" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C225" s="2">
         <v>0.5</v>
@@ -3555,13 +3558,13 @@
     </row>
     <row r="226" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C226" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D226" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3569,13 +3572,13 @@
     </row>
     <row r="227" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
-        <v>1281</v>
+        <v>1278</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C227" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D227" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3583,13 +3586,13 @@
     </row>
     <row r="228" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
-        <v>1282</v>
+        <v>1279</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C228" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="D228" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3597,10 +3600,10 @@
     </row>
     <row r="229" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C229" s="2">
         <v>0.75</v>
@@ -3611,13 +3614,13 @@
     </row>
     <row r="230" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C230" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D230" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3625,13 +3628,13 @@
     </row>
     <row r="231" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
-        <v>1285</v>
+        <v>1282</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C231" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D231" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3639,13 +3642,13 @@
     </row>
     <row r="232" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
-        <v>1286</v>
+        <v>1283</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C232" s="2">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="D232" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3653,10 +3656,10 @@
     </row>
     <row r="233" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
-        <v>1287</v>
+        <v>1284</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C233" s="2">
         <v>0.1</v>
@@ -3667,13 +3670,13 @@
     </row>
     <row r="234" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
-        <v>1288</v>
+        <v>1285</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C234" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D234" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3681,13 +3684,13 @@
     </row>
     <row r="235" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A235" s="2">
-        <v>1289</v>
+        <v>1286</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C235" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D235" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3695,13 +3698,13 @@
     </row>
     <row r="236" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C236" s="2">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="D236" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3709,10 +3712,10 @@
     </row>
     <row r="237" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
-        <v>1291</v>
+        <v>1288</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C237" s="2">
         <v>0.25</v>
@@ -3723,13 +3726,13 @@
     </row>
     <row r="238" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
-        <v>1292</v>
+        <v>1289</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C238" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D238" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3737,13 +3740,13 @@
     </row>
     <row r="239" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
-        <v>1293</v>
+        <v>1290</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C239" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D239" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3751,13 +3754,13 @@
     </row>
     <row r="240" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C240" s="2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D240" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3765,10 +3768,10 @@
     </row>
     <row r="241" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
-        <v>1295</v>
+        <v>1292</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C241" s="2">
         <v>0.4</v>
@@ -3779,13 +3782,13 @@
     </row>
     <row r="242" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
-        <v>1296</v>
+        <v>1293</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C242" s="2">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D242" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3793,13 +3796,13 @@
     </row>
     <row r="243" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C243" s="2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D243" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3807,13 +3810,13 @@
     </row>
     <row r="244" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2">
-        <v>1298</v>
+        <v>1295</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C244" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D244" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3821,13 +3824,13 @@
     </row>
     <row r="245" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="B245" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C245" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D245" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3835,13 +3838,13 @@
     </row>
     <row r="246" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A246" s="2">
-        <v>1300</v>
+        <v>1297</v>
       </c>
       <c r="B246" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C246" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D246" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3849,13 +3852,13 @@
     </row>
     <row r="247" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A247" s="2">
-        <v>1301</v>
+        <v>1298</v>
       </c>
       <c r="B247" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C247" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D247" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3863,13 +3866,13 @@
     </row>
     <row r="248" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2">
-        <v>1302</v>
+        <v>1299</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C248" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D248" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3877,13 +3880,13 @@
     </row>
     <row r="249" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2">
-        <v>1303</v>
+        <v>1300</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C249" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D249" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3891,13 +3894,13 @@
     </row>
     <row r="250" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
-        <v>1304</v>
+        <v>1301</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C250" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D250" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3905,13 +3908,13 @@
     </row>
     <row r="251" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2">
-        <v>1305</v>
+        <v>1302</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C251" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D251" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3919,13 +3922,13 @@
     </row>
     <row r="252" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2">
-        <v>1306</v>
+        <v>1303</v>
       </c>
       <c r="B252" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C252" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D252" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3933,13 +3936,13 @@
     </row>
     <row r="253" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2">
-        <v>1307</v>
+        <v>1304</v>
       </c>
       <c r="B253" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C253" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D253" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3947,13 +3950,13 @@
     </row>
     <row r="254" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C254" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D254" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3961,13 +3964,13 @@
     </row>
     <row r="255" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2">
-        <v>1309</v>
+        <v>1306</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C255" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D255" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3975,13 +3978,13 @@
     </row>
     <row r="256" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2">
-        <v>1310</v>
+        <v>1307</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C256" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D256" s="2">
         <v>2.5700000000000001E-2</v>
@@ -3989,13 +3992,13 @@
     </row>
     <row r="257" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2">
-        <v>1311</v>
+        <v>1308</v>
       </c>
       <c r="B257" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C257" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D257" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4003,13 +4006,13 @@
     </row>
     <row r="258" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2">
-        <v>1312</v>
+        <v>1309</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C258" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D258" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4017,13 +4020,13 @@
     </row>
     <row r="259" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2">
-        <v>1313</v>
+        <v>1310</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C259" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D259" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4031,13 +4034,13 @@
     </row>
     <row r="260" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A260" s="2">
-        <v>1314</v>
+        <v>1311</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C260" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D260" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4045,13 +4048,13 @@
     </row>
     <row r="261" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2">
-        <v>1315</v>
+        <v>1312</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C261" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D261" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4059,13 +4062,13 @@
     </row>
     <row r="262" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2">
-        <v>1316</v>
+        <v>1313</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C262" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D262" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4073,13 +4076,13 @@
     </row>
     <row r="263" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2">
-        <v>1317</v>
+        <v>1314</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C263" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D263" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4087,13 +4090,13 @@
     </row>
     <row r="264" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2">
-        <v>1318</v>
+        <v>1315</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C264" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D264" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4101,13 +4104,13 @@
     </row>
     <row r="265" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C265" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D265" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4115,13 +4118,13 @@
     </row>
     <row r="266" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2">
-        <v>1320</v>
+        <v>1317</v>
       </c>
       <c r="B266" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C266" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D266" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4129,13 +4132,13 @@
     </row>
     <row r="267" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C267" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="D267" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4143,13 +4146,13 @@
     </row>
     <row r="268" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C268" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D268" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4157,13 +4160,13 @@
     </row>
     <row r="269" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2">
-        <v>1323</v>
+        <v>1320</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C269" s="2">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D269" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4171,13 +4174,13 @@
     </row>
     <row r="270" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C270" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="D270" s="2">
         <v>2.5700000000000001E-2</v>
@@ -4185,15 +4188,57 @@
     </row>
     <row r="271" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C271" s="2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D271" s="2">
+        <v>2.5700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="2">
+        <v>1323</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C272" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D272" s="2">
+        <v>2.5700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="2">
+        <v>1324</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C273" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D273" s="2">
+        <v>2.5700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="2">
+        <v>1325</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C274" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="D274" s="2">
         <v>2.5700000000000001E-2</v>
       </c>
     </row>

</xml_diff>